<commit_message>
Add diary ZihuaWeng (#99)
</commit_message>
<xml_diff>
--- a/diaries/diary-ZihuaWeng.xlsx
+++ b/diaries/diary-ZihuaWeng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihuaweng/Documents/study/2019winter/SWE265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FE4DA4-576E-3540-A4B2-F864D6A200AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1722E9-097C-B043-80A4-7E632249EE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -54,39 +54,18 @@
     <t>Participants</t>
   </si>
   <si>
-    <t>&lt;what day?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what time?&gt;</t>
-  </si>
-  <si>
     <t>Reflection</t>
   </si>
   <si>
-    <t>&lt;as applicable, with whom?&gt;</t>
-  </si>
-  <si>
     <t>Your Overall Mood</t>
   </si>
   <si>
     <t>Goal</t>
   </si>
   <si>
-    <t>&lt;what did you want to accomplish?&gt;</t>
-  </si>
-  <si>
     <t>Achievements</t>
   </si>
   <si>
-    <t>&lt;what did you actually accomplish?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;what insight(s) did you gain?&gt;</t>
-  </si>
-  <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
-  </si>
-  <si>
     <t>Zihua Weng</t>
   </si>
   <si>
@@ -105,9 +84,6 @@
     <t>5pm-8pm</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Reverse Engineering introduction. Set up enviroment and get formilar with IntelliJ.</t>
   </si>
   <si>
@@ -115,6 +91,43 @@
   </si>
   <si>
     <t>Gained a bigger view of reverse engineering. Understood more about IntelliJ configuration and debug.</t>
+  </si>
+  <si>
+    <t>Jan 16th</t>
+  </si>
+  <si>
+    <t>Learn how to read code from academic view and industry view.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand different way to debug an exist project. </t>
+  </si>
+  <si>
+    <t>4pm-5pm</t>
+  </si>
+  <si>
+    <t>Junxian, Wenchia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andre, Kaj </t>
+  </si>
+  <si>
+    <t>Andre, Kaj, Ping</t>
+  </si>
+  <si>
+    <t>Build JEdit on Intellij.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build Jedit, and studey Ant, Maven, </t>
+  </si>
+  <si>
+    <t>Error happened when building Jedit using Ant as some dependencies are missing.</t>
+  </si>
+  <si>
+    <t>1. Error happened when building jpacman2 and solved it by redownloading .
+2. For debuging in a project, class names and method names will be useful.</t>
+  </si>
+  <si>
+    <t>Feeling difficult to understand why to use Ant Maven and their difference.</t>
   </si>
 </sst>
 </file>
@@ -279,11 +292,11 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -606,7 +619,7 @@
   <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -615,24 +628,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
@@ -648,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -660,8 +673,8 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>19</v>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -673,8 +686,8 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>20</v>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -711,85 +724,85 @@
         <v>6</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="F11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update diaries/diary-ZihuaWeng.xlsx Jan 20
</commit_message>
<xml_diff>
--- a/diaries/diary-ZihuaWeng.xlsx
+++ b/diaries/diary-ZihuaWeng.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihuaweng/Documents/study/2019winter/SWE265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1722E9-097C-B043-80A4-7E632249EE01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7713F48-7439-1F45-BBD2-89D74E9BC4C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -128,6 +128,42 @@
   </si>
   <si>
     <t>Feeling difficult to understand why to use Ant Maven and their difference.</t>
+  </si>
+  <si>
+    <t>Jan 19th</t>
+  </si>
+  <si>
+    <t>10pm-11.30pm</t>
+  </si>
+  <si>
+    <t>Find a open source project for our coursework as our first choice was disapproved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checked out different Java open sourse project and learn to use IntellJ find the project size. At the end we chose Realm which is a mobile database that frequently used on Android </t>
+  </si>
+  <si>
+    <t>excited!</t>
+  </si>
+  <si>
+    <t>Many popular network framework used on Android do not have a lot code…Eleticsearch is perfect but too big for us...</t>
+  </si>
+  <si>
+    <t>Jan 20th</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Finish homework1</t>
+  </si>
+  <si>
+    <t>Learn to commit and pull request after change multiple documents and after the fork repository got changed.</t>
+  </si>
+  <si>
+    <t>Happy to get my homework done!</t>
+  </si>
+  <si>
+    <t>Finished homework1 and wrote a report using markdown. Refreshed my knowledge of how to write markdown document. Also get more understand of the project Jpacman3, especially the project structure and how the game wrote!</t>
   </si>
 </sst>
 </file>
@@ -618,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -805,23 +841,51 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+    <row r="13" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>

</xml_diff>

<commit_message>
Update Diary Zihua Weng (#276)
* update diary

* update diary
</commit_message>
<xml_diff>
--- a/diaries/diary-ZihuaWeng.xlsx
+++ b/diaries/diary-ZihuaWeng.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihuaweng/Documents/study/2019winter/SWE265P/W2020/diaries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zihuaweng/Documents/study/learning_material/2019winter/SWE265P/W2020/diaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30EBFFE-DD8A-6144-B172-DFF547D5E99C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F86E5F-748A-DC43-8B0E-06DA447720EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -266,6 +266,51 @@
   </si>
   <si>
     <t>Happy to finish the first code reading homework!!!!</t>
+  </si>
+  <si>
+    <t>Learn umls and different code graph</t>
+  </si>
+  <si>
+    <t>Drew different umls and code graph for my code.</t>
+  </si>
+  <si>
+    <t>Working in team is very important! When figuring out a problem, we should work as deep as we need. Try to brainstorm as more possibilities as we can before we head to the final solution. Recruiters are looking for candicates who could tear thing apart and solve problems. We need to make sure we have a clear communication and show how we get a relationship with others when we answer the questions.</t>
+  </si>
+  <si>
+    <t>Cool!</t>
+  </si>
+  <si>
+    <t>Feb 4th</t>
+  </si>
+  <si>
+    <t>8pm-9pm</t>
+  </si>
+  <si>
+    <t>Select two features from Realm for homework 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We decided to look at features: 1. Add methods to table query. 2. Change encryption algorithms </t>
+  </si>
+  <si>
+    <t>Feel like we have a lot work to do to understand the whole project which is well developed within years….</t>
+  </si>
+  <si>
+    <t>Feb 6th</t>
+  </si>
+  <si>
+    <t>Finish homework2. Read the code of the above two features and understand how new developer could modify the code.</t>
+  </si>
+  <si>
+    <t>We finished the first feature1 easily as we know some of the concepts during homework1. But the feature2 is way more difficult as we had difficulty finding the encryption algorithms Realm uses. At the end of the day, everything is executed in C++ and we have hard time chasing the code in deep. Also, I only have littel knowledge of encryption algorithms, so I need to learn more about that later.</t>
+  </si>
+  <si>
+    <t>10am-2pm</t>
+  </si>
+  <si>
+    <t>Finished homework2 and write the report . For the second feature we have trouble finding the encryption algorithm code. Finally, we found out that the default algorithm is AES-256 which is defined in other project called realm-core.</t>
+  </si>
+  <si>
+    <t>It is frustrated that the entryption part of the code is too hard to find and we went to dead end when we chased the code. And a lot project is writen in C++…</t>
   </si>
 </sst>
 </file>
@@ -411,9 +456,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -426,6 +468,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -745,94 +790,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="34.6640625" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="7"/>
+    <col min="1" max="7" width="34.6640625" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
@@ -841,7 +886,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="11"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1119,32 +1164,72 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+    <row r="21" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
@@ -1964,105 +2049,6 @@
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
       <c r="G114" s="4"/>
-    </row>
-    <row r="115" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-      <c r="G115" s="4"/>
-    </row>
-    <row r="116" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
-      <c r="G116" s="4"/>
-    </row>
-    <row r="117" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="4"/>
-    </row>
-    <row r="118" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="4"/>
-    </row>
-    <row r="119" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="4"/>
-    </row>
-    <row r="120" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="4"/>
-    </row>
-    <row r="121" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
-      <c r="G121" s="4"/>
-    </row>
-    <row r="122" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="4"/>
-    </row>
-    <row r="123" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
-      <c r="F123" s="3"/>
-      <c r="G123" s="4"/>
-    </row>
-    <row r="124" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
-      <c r="G124" s="4"/>
-    </row>
-    <row r="125" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A125" s="3"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
-      <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
-      <c r="G125" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>